<commit_message>
Add phase measurement image and update Test.asc parameters
- Added a new phase measurement image (5Hz.png) to the results directory.
- Modified Test.asc to update component values:
  - Changed C1 to 4.7uF and Rc, Cc to 10uF.
  - Adjusted R3 and R4 to 1Meg.
- Updated simulation commands for transient analysis and AC analysis.
- Updated Value Finder.xlsx file.
- Created a temporary file for Value Finder.xlsx.
</commit_message>
<xml_diff>
--- a/Value Finder.xlsx
+++ b/Value Finder.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\Documents\College\Masters\Circuit_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B2925-2308-41A5-9E59-56651EB899EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7107D76A-B275-4B4A-BF3C-C994AD4E709B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{44192CF1-4E54-4094-A156-12815939296E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{44192CF1-4E54-4094-A156-12815939296E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="C_1">Sheet1!$B$7</definedName>
+    <definedName name="C_4">Sheet1!$B$27</definedName>
     <definedName name="C_c">Sheet1!$B$3</definedName>
+    <definedName name="Cap_4">Sheet1!$B$27</definedName>
     <definedName name="Cc">Sheet1!$B$3</definedName>
     <definedName name="F_Lo">Sheet1!$B$1</definedName>
     <definedName name="Gain">Sheet1!$B$4</definedName>
     <definedName name="Lo">Sheet1!$B$1</definedName>
     <definedName name="R_1">Sheet1!$B$5</definedName>
     <definedName name="R_2">Sheet1!$B$6</definedName>
+    <definedName name="R_3">Sheet1!$B$28</definedName>
+    <definedName name="R_4">Sheet1!$B$29</definedName>
     <definedName name="R_c">Sheet1!$B$2</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
@@ -86,7 +90,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -108,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Rc</t>
   </si>
@@ -136,13 +140,52 @@
   <si>
     <t>Capacitors</t>
   </si>
+  <si>
+    <t>OpAmp Cutoff</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Results </t>
+  </si>
+  <si>
+    <t>Av</t>
+  </si>
+  <si>
+    <t>Output Cutoff</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -167,15 +210,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -236,8 +284,8 @@
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="928908" cy="346570"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -279,6 +327,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -417,7 +466,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -481,8 +530,8 @@
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="853887" cy="345672"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -524,6 +573,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -644,7 +694,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -708,8 +758,8 @@
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1351972" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -751,6 +801,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -919,7 +970,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -983,8 +1034,8 @@
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="994503" cy="315792"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1026,6 +1077,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1138,7 +1190,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1194,6 +1246,182 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>315311</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>144517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352934</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>124810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D0DD983-21E7-C103-71EE-20ABAD9324C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2561897" y="1668517"/>
+          <a:ext cx="1870364" cy="1123293"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>243054</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>46555</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>32846</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>72211</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBFBBA9-1A47-0DA2-8580-C066E8719FC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2489640" y="3666055"/>
+          <a:ext cx="1622533" cy="978156"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>157655</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>346650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7477015-DCB6-2014-A256-CD3CD146D438}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9446172" y="183931"/>
+          <a:ext cx="5687219" cy="828791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>197069</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>131379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>281274</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>83827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBCB797B-1176-5BC8-82C2-98020CDAC81C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9485586" y="1083879"/>
+          <a:ext cx="5582429" cy="523948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1514,15 +1742,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F7E90A-6DC5-4F91-AD8A-EC7669570140}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1530,7 +1760,7 @@
         <v>6</v>
       </c>
       <c r="B1">
-        <v>2.3400000000000001E-2</v>
+        <v>1.5900000000000001E-3</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -1563,7 +1793,7 @@
       </c>
       <c r="B3">
         <f>1/(2*PI()*R_c*F_Lo)</f>
-        <v>6.8014932945254415E-7</v>
+        <v>1.0009744848546875E-5</v>
       </c>
       <c r="C3" cm="1">
         <f t="array" ref="C3">SUMPRODUCT((ABS(C_c-$K$2:$K$19)/ABS($K$2:$K$19)&lt;=0.05)*1)</f>
@@ -1581,7 +1811,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I4" s="1">
         <v>10000000</v>
@@ -1613,8 +1843,8 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <f>R_1/2*(Gain-1)</f>
-        <v>9950000</v>
+        <f>(R_1/2)*(Gain-1)</f>
+        <v>10000000</v>
       </c>
       <c r="C6" cm="1">
         <f t="array" ref="C6">SUMPRODUCT((ABS(R_2-$I$2:$I$12)/ABS($I$2:$I$12)&lt;=0.05)*1)</f>
@@ -1633,11 +1863,11 @@
       </c>
       <c r="B7">
         <f>C_c*R_c/(R_1+2*R_2)</f>
-        <v>3.4007466472627207E-7</v>
+        <v>4.9799725614661066E-6</v>
       </c>
       <c r="C7" cm="1">
         <f t="array" ref="C7">SUMPRODUCT((ABS(C_1-$K$2:$K$19)/ABS($K$2:$K$19)&lt;=0.05)*1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
         <v>10000</v>
@@ -1649,7 +1879,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8">
         <f>SUM(C2:C7)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" s="1">
         <v>100000</v>
@@ -1667,6 +1897,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
       <c r="I10" s="1">
         <v>51000</v>
       </c>
@@ -1675,6 +1908,12 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>201</v>
+      </c>
       <c r="I11" s="1">
         <v>330000</v>
       </c>
@@ -1683,6 +1922,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <f>I4*K2</f>
+        <v>6.8</v>
+      </c>
       <c r="I12" s="1">
         <v>6800</v>
       </c>
@@ -1691,11 +1937,25 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <f>K3*(I8+2*I4)</f>
+        <v>6.633</v>
+      </c>
       <c r="K13" s="1">
         <v>3.3000000000000002E-11</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
+        <f>1-B13/B12</f>
+        <v>2.4558823529411744E-2</v>
+      </c>
       <c r="K14" s="1">
         <v>2.1999999999999999E-10</v>
       </c>
@@ -1706,49 +1966,152 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <v>140</v>
+      </c>
       <c r="K16" s="1">
         <v>1E-8</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <f>I4*K2</f>
+        <v>6.8</v>
+      </c>
       <c r="K17" s="1">
         <v>6.8000000000000003E-10</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1">
+        <f>K20*(I8+2*I2)</f>
+        <v>6.4390000000000001</v>
+      </c>
       <c r="K18" s="1">
         <v>2.2000000000000001E-6</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <f>1-B18/B17</f>
+        <v>5.3088235294117658E-2</v>
+      </c>
       <c r="K19" s="1">
         <v>6.7999999999999998E-11</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="1">
+        <v>4.7E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3">
+        <v>100</v>
+      </c>
+      <c r="K21" s="1">
+        <v>6.8000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1">
+        <f>$I$4*$K$2</f>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <f>K7*(I12+2*I11)</f>
+        <v>6.6680000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <f>1-B23/B22</f>
+        <v>1.9411764705882351E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3.3000000000000002E-11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="4">
+        <f>(2*PI()*C_4*R_3)^(-1)</f>
+        <v>4822.8770633907679</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>SUMPRODUCT((ABS(R_c-$I$2:$I$12)/ABS($I$2:$I$12)&lt;=0.05)*1)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>SUMPRODUCT((ABS(C_c-$K$2:$K$20)/ABS($K$2:$K$20)&lt;=0.05)*1)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>SUMPRODUCT((ABS(R_1-$I$2:$I$12)/ABS($I$2:$I$12)&lt;=0.05)*1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>SUMPRODUCT((ABS(R_c-$I$2:$I$12)/ABS($I$2:$I$12)&lt;=0.05)*1)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>SUMPRODUCT((ABS(R_2-$I$2:$I$12)/ABS($I$2:$I$12)&lt;=0.05)*1)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>SUMPRODUCT((ABS(C_c-$K$2:$K$19)/ABS($K$2:$K$19)&lt;=0.05)*1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>SUMPRODUCT((ABS(C_1-$K$2:$K$19)/ABS($K$2:$K$19)&lt;=0.05)*1)&gt;0</formula>
+      <formula>SUMPRODUCT((ABS(C_1-$K$2:$K$20)/ABS($K$2:$K$20)&lt;=0.05)*1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Test.asc parameters and add new Instrument.asc schematic
- Changed frequency parameter in Test.asc from 1 to 100.
- Added new Instrument.asc file containing a detailed schematic with multiple components and connections.
- Updated the Value Finder.xlsx file to reflect changes in component values.
</commit_message>
<xml_diff>
--- a/Value Finder.xlsx
+++ b/Value Finder.xlsx
@@ -8,37 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\Documents\College\Masters\Circuit_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7107D76A-B275-4B4A-BF3C-C994AD4E709B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F751A995-23B1-4151-BAF0-BA5AE1EA4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{44192CF1-4E54-4094-A156-12815939296E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{44192CF1-4E54-4094-A156-12815939296E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Value Finder" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="C_1">Sheet1!$B$7</definedName>
-    <definedName name="C_4">Sheet1!$B$27</definedName>
-    <definedName name="C_c">Sheet1!$B$3</definedName>
-    <definedName name="Cap_4">Sheet1!$B$27</definedName>
-    <definedName name="Cc">Sheet1!$B$3</definedName>
-    <definedName name="F_Lo">Sheet1!$B$1</definedName>
-    <definedName name="Gain">Sheet1!$B$4</definedName>
-    <definedName name="Lo">Sheet1!$B$1</definedName>
-    <definedName name="R_1">Sheet1!$B$5</definedName>
-    <definedName name="R_2">Sheet1!$B$6</definedName>
-    <definedName name="R_3">Sheet1!$B$28</definedName>
-    <definedName name="R_4">Sheet1!$B$29</definedName>
-    <definedName name="R_c">Sheet1!$B$2</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="C_1">'Value Finder'!$B$7</definedName>
+    <definedName name="C_4">'Value Finder'!$B$27</definedName>
+    <definedName name="C_c">'Value Finder'!$B$3</definedName>
+    <definedName name="Cap_4">'Value Finder'!$B$27</definedName>
+    <definedName name="Cc">'Value Finder'!$B$3</definedName>
+    <definedName name="F_Lo">'Value Finder'!$B$1</definedName>
+    <definedName name="Gain">'Value Finder'!$B$4</definedName>
+    <definedName name="Lo">'Value Finder'!$B$1</definedName>
+    <definedName name="R_1">'Value Finder'!$B$5</definedName>
+    <definedName name="R_2">'Value Finder'!$B$6</definedName>
+    <definedName name="R_3">'Value Finder'!$B$28</definedName>
+    <definedName name="R_4">'Value Finder'!$B$29</definedName>
+    <definedName name="R_c">'Value Finder'!$B$2</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Value Finder'!$B$1</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$4</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Value Finder'!$B$1</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Value Finder'!$B$1</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Value Finder'!$B$4</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Value Finder'!$B$4</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
@@ -47,7 +48,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$C$3</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Value Finder'!$C$3</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -68,6 +69,7 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0.00000068</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="Vin">Results!$B$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -112,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Rc</t>
   </si>
@@ -164,6 +166,42 @@
   <si>
     <t>C4</t>
   </si>
+  <si>
+    <t>PHASE ISSUE</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Mistake Result</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Simulated</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Gain(dB)</t>
+  </si>
+  <si>
+    <t>CMMR</t>
+  </si>
+  <si>
+    <t>Vpp</t>
+  </si>
 </sst>
 </file>
 
@@ -214,12 +252,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,6 +313,2260 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Phase Response Simulation vs Measured</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7339-46A0-843A-7246C97A6311}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simulated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7339-46A0-843A-7246C97A6311}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1226720447"/>
+        <c:axId val="1226728127"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1226720447"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1226728127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1226728127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Phase (°)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1226720447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gain Response Simulation vs Measured</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$D$3:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>44.336508465320954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.688614676890388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.10702738893248</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.063921148409776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.063921148409776</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.085501009542568</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.053111079014364</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.889324523231856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B48-4065-B5BB-824DD89A767B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simulated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>44.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.05</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7B48-4065-B5BB-824DD89A767B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1680100735"/>
+        <c:axId val="1680095455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1680100735"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1680095455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1680095455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1680100735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1248,94 +3543,6 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>315311</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>144517</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>352934</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>124810</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D0DD983-21E7-C103-71EE-20ABAD9324C0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2561897" y="1668517"/>
-          <a:ext cx="1870364" cy="1123293"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>243054</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>46555</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>32846</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>72211</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBFBBA9-1A47-0DA2-8580-C066E8719FC6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2489640" y="3666055"/>
-          <a:ext cx="1622533" cy="978156"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>157655</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1361,7 +3568,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1405,7 +3612,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1420,6 +3627,83 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C9E331C-381C-4048-B2F8-26D4399D5739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9AE646A-506C-FB28-01A4-B754E13F5AA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1744,8 +4028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F7E90A-6DC5-4F91-AD8A-EC7669570140}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,8 +4210,8 @@
         <v>6</v>
       </c>
       <c r="B12" s="1">
-        <f>I4*K2</f>
-        <v>6.8</v>
+        <f>I4*K7</f>
+        <v>100.00000000000001</v>
       </c>
       <c r="I12" s="1">
         <v>6800</v>
@@ -1941,8 +4225,8 @@
         <v>9</v>
       </c>
       <c r="B13" s="1">
-        <f>K3*(I8+2*I4)</f>
-        <v>6.633</v>
+        <f>K22*(I8+2*I4)</f>
+        <v>94.47</v>
       </c>
       <c r="K13" s="1">
         <v>3.3000000000000002E-11</v>
@@ -1954,7 +4238,7 @@
       </c>
       <c r="B14" s="2">
         <f>1-B13/B12</f>
-        <v>2.4558823529411744E-2</v>
+        <v>5.5300000000000127E-2</v>
       </c>
       <c r="K14" s="1">
         <v>2.1999999999999999E-10</v>
@@ -1967,11 +4251,9 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3">
-        <v>140</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B16" s="3"/>
       <c r="K16" s="1">
         <v>1E-8</v>
       </c>
@@ -1981,8 +4263,8 @@
         <v>6</v>
       </c>
       <c r="B17" s="1">
-        <f>I4*K2</f>
-        <v>6.8</v>
+        <f>I4*K7</f>
+        <v>100.00000000000001</v>
       </c>
       <c r="K17" s="1">
         <v>6.8000000000000003E-10</v>
@@ -1993,8 +4275,8 @@
         <v>9</v>
       </c>
       <c r="B18" s="1">
-        <f>K20*(I8+2*I2)</f>
-        <v>6.4390000000000001</v>
+        <f>K22*(I8+2*I2)</f>
+        <v>64.39</v>
       </c>
       <c r="K18" s="1">
         <v>2.2000000000000001E-6</v>
@@ -2006,7 +4288,7 @@
       </c>
       <c r="B19" s="2">
         <f>1-B18/B17</f>
-        <v>5.3088235294117658E-2</v>
+        <v>0.35610000000000008</v>
       </c>
       <c r="K19" s="1">
         <v>6.7999999999999998E-11</v>
@@ -2024,6 +4306,9 @@
       <c r="B21" s="3">
         <v>100</v>
       </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
       <c r="K21" s="1">
         <v>6.8000000000000001E-6</v>
       </c>
@@ -2035,6 +4320,9 @@
       <c r="B22" s="1">
         <f>$I$4*$K$2</f>
         <v>6.8</v>
+      </c>
+      <c r="K22" s="1">
+        <v>4.6999999999999999E-6</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2111,11 +4399,357 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>SUMPRODUCT((ABS(C_1-$K$2:$K$20)/ABS($K$2:$K$20)&lt;=0.05)*1)&gt;0</formula>
+      <formula>SUMPRODUCT((ABS(C_1-$K$2:$K$21)/ABS($K$2:$K$21)&lt;=0.05)*1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60205F8B-EA8C-412D-BFD3-5A55E8DC8002}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>6.59</v>
+      </c>
+      <c r="C3">
+        <f>B3/Vin</f>
+        <v>164.75</v>
+      </c>
+      <c r="D3">
+        <f>20*LOG10(C3)</f>
+        <v>44.336508465320954</v>
+      </c>
+      <c r="E3">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="F3">
+        <v>44.4</v>
+      </c>
+      <c r="G3">
+        <v>33.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>7.7</v>
+      </c>
+      <c r="C4">
+        <f>B4/Vin</f>
+        <v>192.5</v>
+      </c>
+      <c r="D4">
+        <f>20*LOG10(C4)</f>
+        <v>45.688614676890388</v>
+      </c>
+      <c r="E4">
+        <v>20.5</v>
+      </c>
+      <c r="F4">
+        <v>45.59</v>
+      </c>
+      <c r="G4">
+        <v>18.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>8.08</v>
+      </c>
+      <c r="C5">
+        <f>B5/Vin</f>
+        <v>202</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D10" si="0">20*LOG10(C5)</f>
+        <v>46.10702738893248</v>
+      </c>
+      <c r="E5">
+        <v>3.7</v>
+      </c>
+      <c r="F5">
+        <v>46.04</v>
+      </c>
+      <c r="G5">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="C6">
+        <f>B6/Vin</f>
+        <v>200.99999999999997</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>46.063921148409776</v>
+      </c>
+      <c r="E6">
+        <v>1.7</v>
+      </c>
+      <c r="F6">
+        <v>46.05</v>
+      </c>
+      <c r="G6">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="C7">
+        <f>B7/Vin</f>
+        <v>200.99999999999997</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>46.063921148409776</v>
+      </c>
+      <c r="E7">
+        <v>-0.3</v>
+      </c>
+      <c r="F7">
+        <v>46.06</v>
+      </c>
+      <c r="G7">
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>8.06</v>
+      </c>
+      <c r="C8">
+        <f>B8/Vin</f>
+        <v>201.5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>46.085501009542568</v>
+      </c>
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>46.06</v>
+      </c>
+      <c r="G8">
+        <v>-1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>150</v>
+      </c>
+      <c r="B9">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="C9">
+        <f>B9/Vin</f>
+        <v>200.74999999999997</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>46.053111079014364</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>46.05</v>
+      </c>
+      <c r="G9">
+        <v>-1.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1000</v>
+      </c>
+      <c r="B10">
+        <v>7.88</v>
+      </c>
+      <c r="C10">
+        <f>B10/Vin</f>
+        <v>197</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>45.889324523231856</v>
+      </c>
+      <c r="E10">
+        <v>-14</v>
+      </c>
+      <c r="F10">
+        <v>45.87</v>
+      </c>
+      <c r="G10">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="e">
+        <f t="shared" ref="C18:C19" si="1">B6/B18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" t="e">
+        <f t="shared" ref="D18:D19" si="2">20*LOG10(C18)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="C20">
+        <f>B7/B20</f>
+        <v>1410.5263157894735</v>
+      </c>
+      <c r="D20">
+        <f>20*LOG10(C20)</f>
+        <v>62.987623861519197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>100</v>
+      </c>
+      <c r="B21">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="C21">
+        <f>B8/B21</f>
+        <v>3100.0000000000005</v>
+      </c>
+      <c r="D21">
+        <f>20*LOG10(C21)</f>
+        <v>69.827233876685455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>150</v>
+      </c>
+      <c r="B22">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="C22">
+        <f>B9/B22</f>
+        <v>3088.4615384615386</v>
+      </c>
+      <c r="D22">
+        <f>20*LOG10(C22)</f>
+        <v>69.794843946157258</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CMRR photos and excel
</commit_message>
<xml_diff>
--- a/Value Finder.xlsx
+++ b/Value Finder.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\Documents\College\Masters\Circuit_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuigalwayie-my.sharepoint.com/personal/b_gillanders1_universityofgalway_ie/Documents/University/Year 5/EE5105/Circuit_Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F751A995-23B1-4151-BAF0-BA5AE1EA4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{F751A995-23B1-4151-BAF0-BA5AE1EA4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C407F37-4B1A-4DDE-A3E1-58665B6D4732}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{44192CF1-4E54-4094-A156-12815939296E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{44192CF1-4E54-4094-A156-12815939296E}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Finder" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="C_1">'Value Finder'!$B$7</definedName>
@@ -22,6 +23,9 @@
     <definedName name="C_c">'Value Finder'!$B$3</definedName>
     <definedName name="Cap_4">'Value Finder'!$B$27</definedName>
     <definedName name="Cc">'Value Finder'!$B$3</definedName>
+    <definedName name="CMRRFreq">Sheet1!$B$1</definedName>
+    <definedName name="CMRRGain">Sheet1!$B$3</definedName>
+    <definedName name="CMRRNoise">Sheet1!$B$2</definedName>
     <definedName name="F_Lo">'Value Finder'!$B$1</definedName>
     <definedName name="Gain">'Value Finder'!$B$4</definedName>
     <definedName name="Lo">'Value Finder'!$B$1</definedName>
@@ -114,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Rc</t>
   </si>
@@ -201,6 +205,54 @@
   </si>
   <si>
     <t>Vpp</t>
+  </si>
+  <si>
+    <t>Input Voltage</t>
+  </si>
+  <si>
+    <t>Output Voltage</t>
+  </si>
+  <si>
+    <t>Frequency (Hz)</t>
+  </si>
+  <si>
+    <t>Noise (V)</t>
+  </si>
+  <si>
+    <t>AbsCMMR</t>
+  </si>
+  <si>
+    <t>CMRR. Without Noise</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>7, 8</t>
+  </si>
+  <si>
+    <t>9, 10</t>
+  </si>
+  <si>
+    <t>11, 12</t>
+  </si>
+  <si>
+    <t>13, 14</t>
+  </si>
+  <si>
+    <t>15, 16</t>
+  </si>
+  <si>
+    <t>17, 18</t>
+  </si>
+  <si>
+    <t>Noise floor</t>
+  </si>
+  <si>
+    <t>19, 20</t>
   </si>
 </sst>
 </file>
@@ -1457,6 +1509,508 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AbsCMMR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>79.455645681425963</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.905224208400696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.120760521565387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.468249216073573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.480296227457274</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.043321235130158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.084521061689401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-07D8-4DD2-8F3F-A522BB9A5CBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMRR. Without Noise</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>80.307886549805261</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.58076416313618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.958471046343661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.958471046343661</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.043321235130151</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-07D8-4DD2-8F3F-A522BB9A5CBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1999269248"/>
+        <c:axId val="1999268288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1999269248"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1999268288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1999268288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1999269248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1537,6 +2091,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2054,6 +2648,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3709,6 +4819,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA87C5F1-F471-E85F-41F5-31494D981167}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4412,7 +5563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60205F8B-EA8C-412D-BFD3-5A55E8DC8002}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -4462,7 +5613,7 @@
         <v>6.59</v>
       </c>
       <c r="C3">
-        <f>B3/Vin</f>
+        <f t="shared" ref="C3:C10" si="0">B3/Vin</f>
         <v>164.75</v>
       </c>
       <c r="D3">
@@ -4487,7 +5638,7 @@
         <v>7.7</v>
       </c>
       <c r="C4">
-        <f>B4/Vin</f>
+        <f t="shared" si="0"/>
         <v>192.5</v>
       </c>
       <c r="D4">
@@ -4512,11 +5663,11 @@
         <v>8.08</v>
       </c>
       <c r="C5">
-        <f>B5/Vin</f>
+        <f t="shared" si="0"/>
         <v>202</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D10" si="0">20*LOG10(C5)</f>
+        <f t="shared" ref="D5:D10" si="1">20*LOG10(C5)</f>
         <v>46.10702738893248</v>
       </c>
       <c r="E5">
@@ -4537,11 +5688,11 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="C6">
-        <f>B6/Vin</f>
+        <f t="shared" si="0"/>
         <v>200.99999999999997</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.063921148409776</v>
       </c>
       <c r="E6">
@@ -4562,11 +5713,11 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="C7">
-        <f>B7/Vin</f>
+        <f t="shared" si="0"/>
         <v>200.99999999999997</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.063921148409776</v>
       </c>
       <c r="E7">
@@ -4587,11 +5738,11 @@
         <v>8.06</v>
       </c>
       <c r="C8">
-        <f>B8/Vin</f>
+        <f t="shared" si="0"/>
         <v>201.5</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.085501009542568</v>
       </c>
       <c r="E8">
@@ -4612,11 +5763,11 @@
         <v>8.0299999999999994</v>
       </c>
       <c r="C9">
-        <f>B9/Vin</f>
+        <f t="shared" si="0"/>
         <v>200.74999999999997</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.053111079014364</v>
       </c>
       <c r="E9">
@@ -4637,11 +5788,11 @@
         <v>7.88</v>
       </c>
       <c r="C10">
-        <f>B10/Vin</f>
+        <f t="shared" si="0"/>
         <v>197</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45.889324523231856</v>
       </c>
       <c r="E10">
@@ -4675,11 +5826,11 @@
         <v>0.5</v>
       </c>
       <c r="C18" t="e">
-        <f t="shared" ref="C18:C19" si="1">B6/B18</f>
+        <f t="shared" ref="C18:C19" si="2">B6/B18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D18" t="e">
-        <f t="shared" ref="D18:D19" si="2">20*LOG10(C18)</f>
+        <f t="shared" ref="D18:D19" si="3">20*LOG10(C18)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4688,11 +5839,11 @@
         <v>10</v>
       </c>
       <c r="C19" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D19" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4752,4 +5903,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905B3796-AAA1-4FCD-B233-5B5106DBF20C}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.107</v>
+      </c>
+      <c r="C5">
+        <f>20*LOG10(CMRRGain/(B5/A5))</f>
+        <v>79.455645681425963</v>
+      </c>
+      <c r="D5">
+        <f>20*LOG10(CMRRGain/((B5-CMRRNoise)/A5))</f>
+        <v>80.307886549805261</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.5</v>
+      </c>
+      <c r="B6">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C6">
+        <f>20*LOG10(CMRRGain/(B6/A6))</f>
+        <v>78.905224208400696</v>
+      </c>
+      <c r="D6">
+        <f>20*LOG10(CMRRGain/((B6-CMRRNoise)/A6))</f>
+        <v>80.58076416313618</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C7">
+        <f>20*LOG10(CMRRGain/(B7/A7))</f>
+        <v>77.120760521565387</v>
+      </c>
+      <c r="D7">
+        <f>20*LOG10(CMRRGain/((B7-CMRRNoise)/A7))</f>
+        <v>80.958471046343661</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C8">
+        <f>20*LOG10(CMRRGain/(B8/A8))</f>
+        <v>74.468249216073573</v>
+      </c>
+      <c r="D8">
+        <f>20*LOG10(CMRRGain/((B8-CMRRNoise)/A8))</f>
+        <v>80.958471046343661</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.1</v>
+      </c>
+      <c r="B9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C9">
+        <f>20*LOG10(CMRRGain/(B9/A9))</f>
+        <v>64.480296227457274</v>
+      </c>
+      <c r="D9">
+        <f>20*LOG10(CMRRGain/((B9-CMRRNoise)/A9))</f>
+        <v>80.043321235130151</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.05</v>
+      </c>
+      <c r="B10">
+        <v>0.01</v>
+      </c>
+      <c r="C10">
+        <f>20*LOG10(CMRRGain/(B10/A10))</f>
+        <v>60.043321235130158</v>
+      </c>
+      <c r="D10" t="e">
+        <f>20*LOG10(CMRRGain/((B10-CMRRNoise)/A10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.02</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+      <c r="C11">
+        <f>20*LOG10(CMRRGain/(B11/A11))</f>
+        <v>52.084521061689401</v>
+      </c>
+      <c r="D11" t="e">
+        <f>20*LOG10(CMRRGain/((B11-CMRRNoise)/A11))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="e">
+        <f>20*LOG10(CMRRGain/(B12/A12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" t="e">
+        <f>20*LOG10(CMRRGain/((B12-CMRRNoise)/A12))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="e">
+        <f>20*LOG10(CMRRGain/(B13/A13))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" t="e">
+        <f>20*LOG10(CMRRGain/((B13-CMRRNoise)/A13))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="e">
+        <f>20*LOG10(CMRRGain/(B14/A14))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" t="e">
+        <f>20*LOG10(CMRRGain/((B14-CMRRNoise)/A14))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="e">
+        <f>20*LOG10(CMRRGain/(B15/A15))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" t="e">
+        <f>20*LOG10(CMRRGain/((B15-CMRRNoise)/A15))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="e">
+        <f>20*LOG10(CMRRGain/(B16/A16))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" t="e">
+        <f>20*LOG10(CMRRGain/((B16-CMRRNoise)/A16))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>